<commit_message>
changed benchmark table rows
</commit_message>
<xml_diff>
--- a/Documantation/benchmark-auswertung.xlsx
+++ b/Documantation/benchmark-auswertung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\HfT\HfT_WS2223\IT-Sicherheit_2\IoT_Crypto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\HfT\HfT_WS2223\IT-Sicherheit_2\IoT_Crypto\dev\Abgabe-Seedorf\Documantation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3F688ED-215E-4E3F-B100-F3EC194018B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57120F-F898-49B7-AABA-110B4474B250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27390" yWindow="-2895" windowWidth="14400" windowHeight="7365" xr2:uid="{3FB04824-2B1A-4172-9DA0-10738A6AE5AD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3FB04824-2B1A-4172-9DA0-10738A6AE5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
   <si>
     <t>Algorithm</t>
   </si>
@@ -371,13 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -386,13 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -402,107 +389,122 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348DB9D0-9DD8-48ED-9215-7617005B9B10}">
-  <dimension ref="A2:H42"/>
+  <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="66" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,566 +832,601 @@
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" customWidth="1"/>
     <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
     <col min="7" max="7" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11" t="s">
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="45" t="s">
+    <row r="6" spans="1:17" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="35">
+        <v>16</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="22">
+      <c r="L7" s="24">
         <v>16</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="M7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="N7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="O7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="P7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="Q7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="26"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19" t="s">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="40">
+        <v>19</v>
+      </c>
+      <c r="F8" s="40">
+        <v>4</v>
+      </c>
+      <c r="G8" s="40">
+        <v>34</v>
+      </c>
+      <c r="H8" s="41">
+        <v>8</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="10">
         <v>571</v>
       </c>
-      <c r="F8" s="20">
+      <c r="O8" s="9">
         <v>118</v>
       </c>
-      <c r="G8" s="19">
+      <c r="P8" s="9">
         <v>1020</v>
       </c>
-      <c r="H8" s="27">
+      <c r="Q8" s="13">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30" t="s">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="44">
+        <v>18</v>
+      </c>
+      <c r="F9" s="44">
+        <v>4</v>
+      </c>
+      <c r="G9" s="44">
+        <v>18</v>
+      </c>
+      <c r="H9" s="45">
+        <v>4</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="14">
         <v>539</v>
       </c>
-      <c r="F9" s="31">
+      <c r="O9" s="14">
         <v>74</v>
       </c>
-      <c r="G9" s="30">
+      <c r="P9" s="14">
         <v>540</v>
       </c>
-      <c r="H9" s="32">
+      <c r="Q9" s="15">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="46" t="s">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11"/>
+      <c r="B11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="27">
+        <v>16</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="33">
+      <c r="L11" s="27">
         <v>16</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="M11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="N11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="O11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="P11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="Q11" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="31"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="46">
+        <v>571</v>
+      </c>
+      <c r="F12" s="8">
+        <v>118</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1020</v>
+      </c>
+      <c r="H12" s="18">
+        <v>234</v>
+      </c>
+      <c r="K12" s="31"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="8">
         <v>19</v>
       </c>
-      <c r="F12" s="16">
+      <c r="O12" s="8">
         <v>4</v>
       </c>
-      <c r="G12" s="15">
+      <c r="P12" s="8">
         <v>34</v>
       </c>
-      <c r="H12" s="38">
+      <c r="Q12" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="19">
+        <v>539</v>
+      </c>
+      <c r="F13" s="19">
+        <v>74</v>
+      </c>
+      <c r="G13" s="19">
+        <v>540</v>
+      </c>
+      <c r="H13" s="20">
+        <v>73</v>
+      </c>
+      <c r="K13" s="32"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="19">
         <v>18</v>
       </c>
-      <c r="F13" s="42">
+      <c r="O13" s="19">
         <v>4</v>
       </c>
-      <c r="G13" s="41">
+      <c r="P13" s="19">
         <v>18</v>
       </c>
-      <c r="H13" s="43">
+      <c r="Q13" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="45" t="s">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="24">
         <v>16</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="26"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19" t="s">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="22"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="9">
         <v>1081</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="9">
         <v>131</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="9">
         <v>1917</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="13">
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="23"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="14">
         <v>1072</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="14">
         <v>165</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="14">
         <v>1070</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="15">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46" t="s">
+    <row r="18" spans="2:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="27">
         <v>24</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="37"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15" t="s">
+    <row r="20" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="31"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="8">
         <v>22</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="8">
         <v>8</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="8">
         <v>41</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="18">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41" t="s">
+    <row r="21" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="32"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="19">
         <v>18</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="19">
         <v>4</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="19">
         <v>18</v>
       </c>
-      <c r="H21" s="43">
+      <c r="H21" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="45" t="s">
+    <row r="22" spans="2:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="24">
         <v>24</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="26"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19" t="s">
+    <row r="24" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="22"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="9">
         <v>601</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="9">
         <v>106</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="9">
         <v>1132</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="13">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30" t="s">
+    <row r="25" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="23"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="14">
         <v>629</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="14">
         <v>128</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="14">
         <v>636</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="15">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="46" t="s">
+    <row r="26" spans="2:8" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="27">
         <v>24</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="37"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15" t="s">
+    <row r="28" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="31"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="8">
         <v>1120</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="8">
         <v>102</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="8">
         <v>2110</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="18">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41" t="s">
+    <row r="29" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="32"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="19">
         <v>1122</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="19">
         <v>126</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="19">
         <v>1128</v>
       </c>
-      <c r="H29" s="43">
+      <c r="H29" s="20">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:8" s="1" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="2:8" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:3" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="2:3" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="2:3" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="2:3" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B15:B17"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>